<commit_message>
Add results for FPGA-based monitor.
Also filled in missing data for filtered/bc sweep.
</commit_message>
<xml_diff>
--- a/figs_src/data_all_hpca.xlsx
+++ b/figs_src/data_all_hpca.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="14850" firstSheet="16" activeTab="18"/>
+    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="14850" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="full_mon" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="69">
   <si>
     <t>DIFT</t>
   </si>
@@ -230,6 +230,30 @@
   <si>
     <t>6 runs</t>
   </si>
+  <si>
+    <t>200m inst instead of 2bn</t>
+  </si>
+  <si>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t>MICRO14 overheads</t>
+  </si>
+  <si>
+    <t>MICRO14 coverage</t>
+  </si>
+  <si>
+    <t>HPCA15 coverage (200m)</t>
+  </si>
+  <si>
+    <t>HPCA15 overheads (200m)</t>
+  </si>
+  <si>
+    <t>HPCA15 overheads (200m inst)</t>
+  </si>
+  <si>
+    <t>HPCA15 coverage (200m inst)</t>
+  </si>
 </sst>
 </file>
 
@@ -267,12 +291,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -291,7 +321,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -316,6 +346,16 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1002,11 +1042,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151750912"/>
-        <c:axId val="151773184"/>
+        <c:axId val="152733952"/>
+        <c:axId val="152756224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151750912"/>
+        <c:axId val="152733952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1015,7 +1055,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151773184"/>
+        <c:crossAx val="152756224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1023,7 +1063,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151773184"/>
+        <c:axId val="152756224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1061,7 +1101,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151750912"/>
+        <c:crossAx val="152733952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1804,11 +1844,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153975808"/>
-        <c:axId val="153977600"/>
+        <c:axId val="155028480"/>
+        <c:axId val="155030272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153975808"/>
+        <c:axId val="155028480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1817,7 +1857,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153977600"/>
+        <c:crossAx val="155030272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1825,7 +1865,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153977600"/>
+        <c:axId val="155030272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1855,7 +1895,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153975808"/>
+        <c:crossAx val="155028480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2294,11 +2334,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="154068864"/>
-        <c:axId val="154070400"/>
+        <c:axId val="155121536"/>
+        <c:axId val="155123072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154068864"/>
+        <c:axId val="155121536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2307,7 +2347,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154070400"/>
+        <c:crossAx val="155123072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2315,7 +2355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154070400"/>
+        <c:axId val="155123072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2339,14 +2379,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154068864"/>
+        <c:crossAx val="155121536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2460,7 +2499,7 @@
                   <c:v>4.7145224509999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9</c:v>
+                  <c:v>3.1125854890000002</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>1.306092995</c:v>
@@ -2518,7 +2557,7 @@
                   <c:v>7.1271726580000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9</c:v>
+                  <c:v>8.256202</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>1.0538627039999999</c:v>
@@ -2573,10 +2612,10 @@
                 <c:formatCode>0.0_);[Red]\(0.0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.9</c:v>
+                  <c:v>4.958189</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9</c:v>
+                  <c:v>5.3545119999999997</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>1.0602838000000001</c:v>
@@ -2692,7 +2731,7 @@
                   <c:v>4.6564346859999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9</c:v>
+                  <c:v>5.7836189999999998</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>1.1280897160000001</c:v>
@@ -2750,7 +2789,7 @@
                   <c:v>4.7046409450000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9</c:v>
+                  <c:v>3.7457660000000002</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>1.1712283459999999</c:v>
@@ -2924,7 +2963,7 @@
                   <c:v>5.6462669849999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9</c:v>
+                  <c:v>4.9528981859999996</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>1.0667325050000001</c:v>
@@ -2979,10 +3018,10 @@
                 <c:formatCode>0.0_);[Red]\(0.0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.5624491840987074</c:v>
+                  <c:v>4.3061679423933619</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9</c:v>
+                  <c:v>3.1392869378396293</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>1.098458793150149</c:v>
@@ -3000,11 +3039,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151850368"/>
-        <c:axId val="151864448"/>
+        <c:axId val="152837504"/>
+        <c:axId val="152847488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151850368"/>
+        <c:axId val="152837504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3013,7 +3052,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151864448"/>
+        <c:crossAx val="152847488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3021,10 +3060,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151864448"/>
+        <c:axId val="152847488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="8"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3060,7 +3098,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151850368"/>
+        <c:crossAx val="152837504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3208,7 +3246,7 @@
                   <c:v>0.5242</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.73089999999999999</c:v>
+                  <c:v>0.77649999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.94399999999999995</c:v>
@@ -3217,7 +3255,7 @@
                   <c:v>0.97319999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.57650000000000001</c:v>
+                  <c:v>0.81679999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -3229,7 +3267,7 @@
                   <c:v>0.77370000000000005</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.82188888888888889</c:v>
+                  <c:v>0.85365555555555561</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3308,7 +3346,7 @@
                   <c:v>0.54790000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.79730000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.9466</c:v>
@@ -3317,7 +3355,7 @@
                   <c:v>0.98119999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.58309999999999995</c:v>
+                  <c:v>0.84199999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -3329,7 +3367,7 @@
                   <c:v>0.79710000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.75128888888888889</c:v>
+                  <c:v>0.86864444444444444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3408,7 +3446,7 @@
                   <c:v>0.57989999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81200000000000006</c:v>
+                  <c:v>0.83620000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -3417,7 +3455,7 @@
                   <c:v>0.98370000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.60499999999999998</c:v>
+                  <c:v>0.87960000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -3429,7 +3467,7 @@
                   <c:v>0.81840000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.85984444444444441</c:v>
+                  <c:v>0.89304444444444442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3508,7 +3546,7 @@
                   <c:v>0.67759999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.95020000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -3517,7 +3555,7 @@
                   <c:v>0.99070000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.66169999999999995</c:v>
+                  <c:v>0.98919999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -3529,7 +3567,7 @@
                   <c:v>0.89059999999999995</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.80218888888888895</c:v>
+                  <c:v>0.94415555555555564</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3617,7 +3655,7 @@
                   <c:v>0.99529999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.71530000000000005</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -3629,7 +3667,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.94521111111111111</c:v>
+                  <c:v>0.97684444444444429</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3717,7 +3755,7 @@
                   <c:v>0.999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.76729999999999998</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -3729,7 +3767,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.0000">
-                  <c:v>0.96740000000000004</c:v>
+                  <c:v>0.99325555555555545</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3744,11 +3782,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153007616"/>
-        <c:axId val="153009152"/>
+        <c:axId val="154056192"/>
+        <c:axId val="154057728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153007616"/>
+        <c:axId val="154056192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3768,7 +3806,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153009152"/>
+        <c:crossAx val="154057728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3776,7 +3814,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153009152"/>
+        <c:axId val="154057728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3814,7 +3852,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153007616"/>
+        <c:crossAx val="154056192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4488,11 +4526,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153247104"/>
-        <c:axId val="153257088"/>
+        <c:axId val="154295680"/>
+        <c:axId val="154305664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153247104"/>
+        <c:axId val="154295680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4512,7 +4550,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153257088"/>
+        <c:crossAx val="154305664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4520,7 +4558,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153257088"/>
+        <c:axId val="154305664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4544,13 +4582,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153247104"/>
+        <c:crossAx val="154295680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5024,11 +5063,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153199744"/>
-        <c:axId val="153201280"/>
+        <c:axId val="154248704"/>
+        <c:axId val="154250240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153199744"/>
+        <c:axId val="154248704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5048,7 +5087,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153201280"/>
+        <c:crossAx val="154250240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5056,7 +5095,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153201280"/>
+        <c:axId val="154250240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5084,13 +5123,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153199744"/>
+        <c:crossAx val="154248704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5211,7 +5251,7 @@
                   <c:v>h264ref</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>average</c:v>
+                  <c:v>geomean</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5220,7 +5260,7 @@
             <c:numRef>
               <c:f>bc_policies!$B$2:$K$2</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.91379999999999995</c:v>
@@ -5249,8 +5289,8 @@
                 <c:pt idx="8">
                   <c:v>0.78669999999999995</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.83</c:v>
+                <c:pt idx="9" formatCode="0%">
+                  <c:v>0.81503135115597636</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5311,7 +5351,7 @@
                   <c:v>h264ref</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>average</c:v>
+                  <c:v>geomean</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5320,7 +5360,7 @@
             <c:numRef>
               <c:f>bc_policies!$B$3:$K$3</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.91190000000000004</c:v>
@@ -5349,8 +5389,8 @@
                 <c:pt idx="8">
                   <c:v>0.81559999999999999</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.92</c:v>
+                <c:pt idx="9" formatCode="0%">
+                  <c:v>0.9136389686081553</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5365,11 +5405,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153497984"/>
-        <c:axId val="153499520"/>
+        <c:axId val="154614016"/>
+        <c:axId val="154615808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153497984"/>
+        <c:axId val="154614016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5378,7 +5418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153499520"/>
+        <c:crossAx val="154615808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5386,7 +5426,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153499520"/>
+        <c:axId val="154615808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5410,13 +5450,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153497984"/>
+        <c:crossAx val="154614016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5689,11 +5730,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153511040"/>
-        <c:axId val="153512576"/>
+        <c:axId val="154657920"/>
+        <c:axId val="154659456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153511040"/>
+        <c:axId val="154657920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5702,7 +5743,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="153512576"/>
+        <c:crossAx val="154659456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5710,7 +5751,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153512576"/>
+        <c:axId val="154659456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.60000000000000009"/>
@@ -5735,13 +5776,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153511040"/>
+        <c:crossAx val="154657920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5863,7 +5905,7 @@
                   <c:v>h264ref</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>average</c:v>
+                  <c:v>geomean</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5875,34 +5917,34 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.91379999999999995</c:v>
+                  <c:v>0.43049999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.53779999999999994</c:v>
+                  <c:v>0.22689999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75449999999999995</c:v>
+                  <c:v>0.44140000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98899999999999999</c:v>
+                  <c:v>0.82330000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.96160000000000001</c:v>
+                  <c:v>0.39529999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.58260000000000001</c:v>
+                  <c:v>0.4148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.49149999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.9819</c:v>
+                  <c:v>0.97660000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.78669999999999995</c:v>
+                  <c:v>0.3533</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.83</c:v>
+                  <c:v>0.46348812893673524</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5963,7 +6005,7 @@
                   <c:v>h264ref</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>average</c:v>
+                  <c:v>geomean</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5975,34 +6017,34 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.91190000000000004</c:v>
+                  <c:v>0.46389999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.81569999999999998</c:v>
+                  <c:v>0.27129999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.73550000000000004</c:v>
+                  <c:v>0.47710000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99739999999999995</c:v>
+                  <c:v>0.79049999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.99990000000000001</c:v>
+                  <c:v>0.42049999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99680000000000002</c:v>
+                  <c:v>0.44019999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.49159999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0.97660000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.81559999999999999</c:v>
+                  <c:v>0.37880000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.92</c:v>
+                  <c:v>0.48897001622478758</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6017,11 +6059,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153118208"/>
-        <c:axId val="153119744"/>
+        <c:axId val="154170880"/>
+        <c:axId val="154172416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153118208"/>
+        <c:axId val="154170880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6030,7 +6072,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153119744"/>
+        <c:crossAx val="154172416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6038,7 +6080,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153119744"/>
+        <c:axId val="154172416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6062,13 +6104,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153118208"/>
+        <c:crossAx val="154170880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6331,11 +6374,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153792896"/>
-        <c:axId val="153794432"/>
+        <c:axId val="154845568"/>
+        <c:axId val="154847104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153792896"/>
+        <c:axId val="154845568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6344,7 +6387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="153794432"/>
+        <c:crossAx val="154847104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6352,7 +6395,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153794432"/>
+        <c:axId val="154847104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6375,13 +6418,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153792896"/>
+        <c:crossAx val="154845568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6441,7 +6485,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="266" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="325" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" r:id="rId1"/>
@@ -6477,7 +6521,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="147" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="158" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="159" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6489,7 +6533,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="147" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="158" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="159" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6501,7 +6545,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="147" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="160" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="159" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6513,7 +6557,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="285" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="298" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6525,7 +6569,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="285" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="298" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6537,7 +6581,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="285" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="298" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6549,7 +6593,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="285" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="298" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6561,7 +6605,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="3081338" cy="2176463"/>
+    <xdr:ext cx="2928938" cy="2024063"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6588,7 +6632,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="2927684" cy="2028658"/>
+    <xdr:ext cx="2927819" cy="2026460"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6615,7 +6659,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="3083092" cy="2180724"/>
+    <xdr:ext cx="2927838" cy="2028092"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6696,7 +6740,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6285204" cy="2183622"/>
+    <xdr:ext cx="6124937" cy="2025570"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6723,7 +6767,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6285204" cy="2183622"/>
+    <xdr:ext cx="6124937" cy="2025570"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6750,7 +6794,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6285204" cy="2183622"/>
+    <xdr:ext cx="6125766" cy="2024063"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6777,7 +6821,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="2927684" cy="2028658"/>
+    <xdr:ext cx="2927819" cy="2026460"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6804,7 +6848,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="2927684" cy="2028658"/>
+    <xdr:ext cx="2927819" cy="2026460"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -7087,7 +7131,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="2927684" cy="2028658"/>
+    <xdr:ext cx="2927819" cy="2026460"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -9315,7 +9359,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -9368,8 +9412,8 @@
       <c r="C2" s="3">
         <v>7.1271726580000001</v>
       </c>
-      <c r="D2" s="3">
-        <v>0.9</v>
+      <c r="D2" s="16">
+        <v>4.958189</v>
       </c>
       <c r="E2" s="3">
         <v>1.745944962</v>
@@ -9391,11 +9435,11 @@
       </c>
       <c r="K2" s="2">
         <f>GEOMEAN(B2:J2)</f>
-        <v>3.5624491840987074</v>
+        <v>4.3061679423933619</v>
       </c>
       <c r="L2" s="5">
         <f>MIN(B2:J2)</f>
-        <v>0.9</v>
+        <v>1.745944962</v>
       </c>
       <c r="M2" s="5">
         <f>MAX(B2:J2)</f>
@@ -9407,22 +9451,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.9</v>
+        <v>3.1125854890000002</v>
+      </c>
+      <c r="C3" s="16">
+        <v>8.256202</v>
+      </c>
+      <c r="D3" s="16">
+        <v>5.3545119999999997</v>
       </c>
       <c r="E3" s="3">
         <v>1.550173698</v>
       </c>
-      <c r="F3" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.9</v>
+      <c r="F3" s="16">
+        <v>5.7836189999999998</v>
+      </c>
+      <c r="G3" s="16">
+        <v>3.7457660000000002</v>
       </c>
       <c r="H3" s="3">
         <v>1.0804225220000001</v>
@@ -9431,18 +9475,19 @@
         <v>1.1975231289999999</v>
       </c>
       <c r="J3" s="3">
-        <v>0.9</v>
+        <v>4.9528981859999996</v>
       </c>
       <c r="K3" s="2">
-        <v>0.9</v>
+        <f>GEOMEAN(B3:J3)</f>
+        <v>3.1392869378396293</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" ref="L3:L4" si="0">MIN(B3:J3)</f>
-        <v>0.9</v>
+        <v>1.0804225220000001</v>
       </c>
       <c r="M3" s="5">
         <f t="shared" ref="M3:M4" si="1">MAX(B3:J3)</f>
-        <v>1.550173698</v>
+        <v>8.256202</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -9539,15 +9584,18 @@
       </c>
     </row>
     <row r="8" spans="1:13">
+      <c r="A8" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="K8" s="8">
         <f>1-K2/full_mon!K2</f>
-        <v>0.65038422202265278</v>
+        <v>0.57739628624012007</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="K9" s="8">
         <f>1-K3/full_mon!K3</f>
-        <v>0.94261379343507645</v>
+        <v>0.79983136813174327</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -9569,10 +9617,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -9622,8 +9670,8 @@
       <c r="C2" s="11">
         <v>0.5242</v>
       </c>
-      <c r="D2" s="11">
-        <v>0.73089999999999999</v>
+      <c r="D2" s="18">
+        <v>0.77649999999999997</v>
       </c>
       <c r="E2" s="11">
         <v>0.94399999999999995</v>
@@ -9631,8 +9679,8 @@
       <c r="F2" s="11">
         <v>0.97319999999999995</v>
       </c>
-      <c r="G2" s="11">
-        <v>0.57650000000000001</v>
+      <c r="G2" s="18">
+        <v>0.81679999999999997</v>
       </c>
       <c r="H2" s="11">
         <v>1</v>
@@ -9645,7 +9693,7 @@
       </c>
       <c r="K2" s="10">
         <f>AVERAGE(B2:J2)</f>
-        <v>0.82188888888888889</v>
+        <v>0.85365555555555561</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -9658,8 +9706,8 @@
       <c r="C3" s="11">
         <v>0.54790000000000005</v>
       </c>
-      <c r="D3" s="11">
-        <v>0</v>
+      <c r="D3" s="18">
+        <v>0.79730000000000001</v>
       </c>
       <c r="E3" s="11">
         <v>0.9466</v>
@@ -9667,8 +9715,8 @@
       <c r="F3" s="11">
         <v>0.98119999999999996</v>
       </c>
-      <c r="G3" s="11">
-        <v>0.58309999999999995</v>
+      <c r="G3" s="18">
+        <v>0.84199999999999997</v>
       </c>
       <c r="H3" s="11">
         <v>1</v>
@@ -9681,7 +9729,7 @@
       </c>
       <c r="K3" s="10">
         <f t="shared" ref="K3:K7" si="0">AVERAGE(B3:J3)</f>
-        <v>0.75128888888888889</v>
+        <v>0.86864444444444444</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -9694,8 +9742,8 @@
       <c r="C4" s="11">
         <v>0.57989999999999997</v>
       </c>
-      <c r="D4" s="11">
-        <v>0.81200000000000006</v>
+      <c r="D4" s="18">
+        <v>0.83620000000000005</v>
       </c>
       <c r="E4" s="11">
         <v>1</v>
@@ -9703,8 +9751,8 @@
       <c r="F4" s="11">
         <v>0.98370000000000002</v>
       </c>
-      <c r="G4" s="11">
-        <v>0.60499999999999998</v>
+      <c r="G4" s="18">
+        <v>0.87960000000000005</v>
       </c>
       <c r="H4" s="11">
         <v>1</v>
@@ -9717,7 +9765,7 @@
       </c>
       <c r="K4" s="10">
         <f t="shared" si="0"/>
-        <v>0.85984444444444441</v>
+        <v>0.89304444444444442</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -9730,8 +9778,8 @@
       <c r="C5" s="11">
         <v>0.67759999999999998</v>
       </c>
-      <c r="D5" s="11">
-        <v>0</v>
+      <c r="D5" s="18">
+        <v>0.95020000000000004</v>
       </c>
       <c r="E5" s="11">
         <v>1</v>
@@ -9739,8 +9787,8 @@
       <c r="F5" s="11">
         <v>0.99070000000000003</v>
       </c>
-      <c r="G5" s="11">
-        <v>0.66169999999999995</v>
+      <c r="G5" s="18">
+        <v>0.98919999999999997</v>
       </c>
       <c r="H5" s="11">
         <v>1</v>
@@ -9753,7 +9801,7 @@
       </c>
       <c r="K5" s="10">
         <f t="shared" si="0"/>
-        <v>0.80218888888888895</v>
+        <v>0.94415555555555564</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -9766,7 +9814,7 @@
       <c r="C6" s="11">
         <v>0.79630000000000001</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="18">
         <v>1</v>
       </c>
       <c r="E6" s="11">
@@ -9775,8 +9823,8 @@
       <c r="F6" s="11">
         <v>0.99529999999999996</v>
       </c>
-      <c r="G6" s="11">
-        <v>0.71530000000000005</v>
+      <c r="G6" s="18">
+        <v>1</v>
       </c>
       <c r="H6" s="11">
         <v>1</v>
@@ -9789,7 +9837,7 @@
       </c>
       <c r="K6" s="10">
         <f t="shared" si="0"/>
-        <v>0.94521111111111111</v>
+        <v>0.97684444444444429</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -9802,7 +9850,7 @@
       <c r="C7" s="11">
         <v>0.94030000000000002</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="18">
         <v>1</v>
       </c>
       <c r="E7" s="11">
@@ -9811,8 +9859,8 @@
       <c r="F7" s="11">
         <v>0.999</v>
       </c>
-      <c r="G7" s="11">
-        <v>0.76729999999999998</v>
+      <c r="G7" s="18">
+        <v>1</v>
       </c>
       <c r="H7" s="11">
         <v>1</v>
@@ -9825,14 +9873,14 @@
       </c>
       <c r="K7" s="10">
         <f t="shared" si="0"/>
-        <v>0.96740000000000004</v>
+        <v>0.99325555555555545</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="8"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -9845,14 +9893,58 @@
       <c r="A9" s="8"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="D9" s="11">
+        <v>0.73089999999999999</v>
+      </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="G9" s="11">
+        <v>0.57650000000000001</v>
+      </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
       <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0.58309999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="D11" s="11">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0.60499999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="D12" s="11">
+        <v>0</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0.66169999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="D13" s="11">
+        <v>1</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0.71530000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="D14" s="11">
+        <v>1</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0.76729999999999998</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10501,15 +10593,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -10538,7 +10633,7 @@
         <v>4</v>
       </c>
       <c r="K1" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="L1" t="s">
         <v>23</v>
@@ -10551,40 +10646,43 @@
       <c r="A2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="14">
         <v>0.91379999999999995</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="14">
         <v>0.53779999999999994</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="14">
         <v>0.75449999999999995</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="14">
         <v>0.98899999999999999</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="14">
         <v>0.96160000000000001</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="14">
         <v>0.58260000000000001</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="14">
         <v>1</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="14">
         <v>0.9819</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="14">
         <v>0.78669999999999995</v>
       </c>
       <c r="K2" s="8">
-        <v>0.83</v>
+        <f>GEOMEAN(B2:J2)</f>
+        <v>0.81503135115597636</v>
       </c>
       <c r="L2" s="8">
-        <v>0.54</v>
+        <f>MIN(B2:J2)</f>
+        <v>0.53779999999999994</v>
       </c>
       <c r="M2" s="8">
+        <f>MAX(B2:J2)</f>
         <v>1</v>
       </c>
     </row>
@@ -10592,40 +10690,43 @@
       <c r="A3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="14">
         <v>0.91190000000000004</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="14">
         <v>0.81569999999999998</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="14">
         <v>0.73550000000000004</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="14">
         <v>0.99739999999999995</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="14">
         <v>0.99990000000000001</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="14">
         <v>0.99680000000000002</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="14">
         <v>1</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="14">
         <v>1</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="14">
         <v>0.81559999999999999</v>
       </c>
       <c r="K3" s="8">
-        <v>0.92</v>
+        <f>GEOMEAN(B3:J3)</f>
+        <v>0.9136389686081553</v>
       </c>
       <c r="L3" s="8">
-        <v>0.74</v>
+        <f>MIN(B3:J3)</f>
+        <v>0.73550000000000004</v>
       </c>
       <c r="M3" s="8">
+        <f>MAX(B3:J3)</f>
         <v>1</v>
       </c>
     </row>
@@ -10702,12 +10803,15 @@
         <v>-5.0000000000000001E-4</v>
       </c>
       <c r="K6" s="9">
-        <v>-0.16</v>
+        <f>AVERAGE(B6:J6)</f>
+        <v>-0.15747777777777777</v>
       </c>
       <c r="L6" s="8">
-        <v>-0.47</v>
+        <f>MIN(B6:J6)</f>
+        <v>-0.46989999999999998</v>
       </c>
       <c r="M6" s="8">
+        <f>MAX(B6:J6)</f>
         <v>0.04</v>
       </c>
     </row>
@@ -10743,13 +10847,268 @@
         <v>0.10340000000000001</v>
       </c>
       <c r="K7" s="9">
-        <v>2.2200000000000002</v>
+        <f>AVERAGE(B7:J7)</f>
+        <v>2.2157888888888895</v>
       </c>
       <c r="L7" s="8">
-        <v>-0.44</v>
+        <f>MIN(B7:J7)</f>
+        <v>-0.44119999999999998</v>
       </c>
       <c r="M7" s="8">
-        <v>15.14</v>
+        <f>MAX(B7:J7)</f>
+        <v>15.1409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="B11" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="C11" s="9">
+        <v>-9.6000000000000002E-2</v>
+      </c>
+      <c r="D11" s="9">
+        <v>-1.7899999999999999E-2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>-0.38080000000000003</v>
+      </c>
+      <c r="F11" s="9">
+        <v>-5.3199999999999997E-2</v>
+      </c>
+      <c r="G11" s="9">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="H11" s="9">
+        <v>-0.44119999999999998</v>
+      </c>
+      <c r="I11" s="9">
+        <v>-0.46989999999999998</v>
+      </c>
+      <c r="J11" s="9">
+        <v>-5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="B12" s="9">
+        <v>0.2697</v>
+      </c>
+      <c r="C12" s="9">
+        <v>4.1905999999999999</v>
+      </c>
+      <c r="D12" s="9">
+        <v>-1.8499999999999999E-2</v>
+      </c>
+      <c r="E12" s="9">
+        <v>-0.29210000000000003</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1.1740999999999999</v>
+      </c>
+      <c r="G12" s="9">
+        <v>15.1409</v>
+      </c>
+      <c r="H12" s="9">
+        <v>-0.44119999999999998</v>
+      </c>
+      <c r="I12" s="9">
+        <v>-0.18479999999999999</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0.10340000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="B14" s="14">
+        <v>0.91379999999999995</v>
+      </c>
+      <c r="C14" s="14">
+        <v>0.53779999999999994</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0.75449999999999995</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0.96160000000000001</v>
+      </c>
+      <c r="G14" s="14">
+        <v>0.58260000000000001</v>
+      </c>
+      <c r="H14" s="14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="14">
+        <v>0.9819</v>
+      </c>
+      <c r="J14" s="14">
+        <v>0.78669999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15" s="14">
+        <v>0.91190000000000004</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0.81569999999999998</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0.73550000000000004</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.99739999999999995</v>
+      </c>
+      <c r="F15" s="14">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G15" s="14">
+        <v>0.99680000000000002</v>
+      </c>
+      <c r="H15" s="14">
+        <v>1</v>
+      </c>
+      <c r="I15" s="14">
+        <v>1</v>
+      </c>
+      <c r="J15" s="14">
+        <v>0.81559999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="B17" s="9">
+        <v>4.4506527999999997E-2</v>
+      </c>
+      <c r="C17" s="9">
+        <v>-0.29935793399999999</v>
+      </c>
+      <c r="D17" s="9">
+        <v>3.600838E-2</v>
+      </c>
+      <c r="E17" s="9">
+        <v>-0.12163595100000001</v>
+      </c>
+      <c r="F17" s="9">
+        <v>-3.3307832000000002E-2</v>
+      </c>
+      <c r="G17" s="9">
+        <v>-6.1883876999999997E-2</v>
+      </c>
+      <c r="H17" s="9">
+        <v>-0.493118212</v>
+      </c>
+      <c r="I17" s="9">
+        <v>-0.37364656899999998</v>
+      </c>
+      <c r="J17" s="9">
+        <v>4.4596485999999998E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="9">
+        <v>5.4728245000000002E-2</v>
+      </c>
+      <c r="C18" s="9">
+        <v>6.7562023790000003</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.108630981</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0.149038591</v>
+      </c>
+      <c r="F18" s="9">
+        <v>4.38289185</v>
+      </c>
+      <c r="G18" s="9">
+        <v>2.2387061849999998</v>
+      </c>
+      <c r="H18" s="9">
+        <v>-0.493118212</v>
+      </c>
+      <c r="I18" s="9">
+        <v>1.091423579</v>
+      </c>
+      <c r="J18" s="9">
+        <v>-0.34753614799999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="B20" s="8">
+        <v>0.88780000000000003</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0.47749999999999998</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0.79730000000000001</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0.97529999999999994</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0.81740000000000002</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="H20" s="8">
+        <v>1</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0.92030000000000001</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0.78080000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="B21" s="8">
+        <v>0.87339999999999995</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0.80779999999999996</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0.98819999999999997</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0.99970000000000003</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.99919999999999998</v>
+      </c>
+      <c r="H21" s="8">
+        <v>1</v>
+      </c>
+      <c r="I21" s="8">
+        <v>1</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0.76139999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -10759,10 +11118,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10796,7 +11155,7 @@
         <v>4</v>
       </c>
       <c r="K1" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="L1" t="s">
         <v>23</v>
@@ -10810,40 +11169,43 @@
         <v>30</v>
       </c>
       <c r="B2" s="8">
-        <v>0.91379999999999995</v>
+        <v>0.43049999999999999</v>
       </c>
       <c r="C2" s="8">
-        <v>0.53779999999999994</v>
+        <v>0.22689999999999999</v>
       </c>
       <c r="D2" s="8">
-        <v>0.75449999999999995</v>
+        <v>0.44140000000000001</v>
       </c>
       <c r="E2" s="8">
-        <v>0.98899999999999999</v>
+        <v>0.82330000000000003</v>
       </c>
       <c r="F2" s="8">
-        <v>0.96160000000000001</v>
+        <v>0.39529999999999998</v>
       </c>
       <c r="G2" s="8">
-        <v>0.58260000000000001</v>
+        <v>0.4148</v>
       </c>
       <c r="H2" s="8">
-        <v>1</v>
+        <v>0.49149999999999999</v>
       </c>
       <c r="I2" s="8">
-        <v>0.9819</v>
+        <v>0.97660000000000002</v>
       </c>
       <c r="J2" s="8">
-        <v>0.78669999999999995</v>
+        <v>0.3533</v>
       </c>
       <c r="K2" s="8">
-        <v>0.83</v>
+        <f>GEOMEAN(B2:J2)</f>
+        <v>0.46348812893673524</v>
       </c>
       <c r="L2" s="8">
-        <v>0.54</v>
+        <f>MIN(B2:J2)</f>
+        <v>0.22689999999999999</v>
       </c>
       <c r="M2" s="8">
-        <v>1</v>
+        <f>MAX(B2:J2)</f>
+        <v>0.97660000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -10851,40 +11213,43 @@
         <v>29</v>
       </c>
       <c r="B3" s="8">
-        <v>0.91190000000000004</v>
+        <v>0.46389999999999998</v>
       </c>
       <c r="C3" s="8">
-        <v>0.81569999999999998</v>
+        <v>0.27129999999999999</v>
       </c>
       <c r="D3" s="8">
-        <v>0.73550000000000004</v>
+        <v>0.47710000000000002</v>
       </c>
       <c r="E3" s="8">
-        <v>0.99739999999999995</v>
+        <v>0.79049999999999998</v>
       </c>
       <c r="F3" s="8">
-        <v>0.99990000000000001</v>
+        <v>0.42049999999999998</v>
       </c>
       <c r="G3" s="8">
-        <v>0.99680000000000002</v>
+        <v>0.44019999999999998</v>
       </c>
       <c r="H3" s="8">
-        <v>1</v>
+        <v>0.49159999999999998</v>
       </c>
       <c r="I3" s="8">
-        <v>1</v>
+        <v>0.97660000000000002</v>
       </c>
       <c r="J3" s="8">
-        <v>0.81559999999999999</v>
+        <v>0.37880000000000003</v>
       </c>
       <c r="K3" s="8">
-        <v>0.92</v>
+        <f>GEOMEAN(B3:J3)</f>
+        <v>0.48897001622478758</v>
       </c>
       <c r="L3" s="8">
-        <v>0.74</v>
+        <f>MIN(B3:J3)</f>
+        <v>0.27129999999999999</v>
       </c>
       <c r="M3" s="8">
-        <v>1</v>
+        <f>MAX(B3:J3)</f>
+        <v>0.97660000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -10972,13 +11337,16 @@
         <v>9.5999999999999992E-3</v>
       </c>
       <c r="K6" s="8">
-        <v>-0.05</v>
+        <f>AVERAGE(B6:J6)</f>
+        <v>-4.9188888888888886E-2</v>
       </c>
       <c r="L6" s="8">
-        <v>-0.19</v>
+        <f>MIN(B6:J6)</f>
+        <v>-0.18629999999999999</v>
       </c>
       <c r="M6" s="8">
-        <v>0.01</v>
+        <f>MAX(B6:J6)</f>
+        <v>1.15E-2</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -11013,13 +11381,268 @@
         <v>9.7000000000000003E-3</v>
       </c>
       <c r="K7" s="8">
-        <v>-0.05</v>
+        <f>AVERAGE(B7:J7)</f>
+        <v>-5.0588888888888885E-2</v>
       </c>
       <c r="L7" s="8">
-        <v>-0.19</v>
+        <f>MIN(B7:J7)</f>
+        <v>-0.186</v>
       </c>
       <c r="M7" s="8">
-        <v>0.01</v>
+        <f>MAX(B7:J7)</f>
+        <v>1.1900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="B12" s="8">
+        <v>0.43049999999999999</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.22689999999999999</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.44140000000000001</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.82330000000000003</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.39529999999999998</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.4148</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0.49149999999999999</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.97660000000000002</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0.3533</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="B13" s="8">
+        <v>0.46389999999999998</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.27129999999999999</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.47710000000000002</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.79049999999999998</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.42049999999999998</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.44019999999999998</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0.49159999999999998</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0.97660000000000002</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.37880000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15" s="8">
+        <v>1.15E-2</v>
+      </c>
+      <c r="C15" s="8">
+        <v>-6.6600000000000006E-2</v>
+      </c>
+      <c r="D15" s="8">
+        <v>-6.8999999999999999E-3</v>
+      </c>
+      <c r="E15" s="8">
+        <v>-0.10630000000000001</v>
+      </c>
+      <c r="F15" s="8">
+        <v>-1.09E-2</v>
+      </c>
+      <c r="G15" s="8">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="H15" s="8">
+        <v>-0.18629999999999999</v>
+      </c>
+      <c r="I15" s="8">
+        <v>-8.2799999999999999E-2</v>
+      </c>
+      <c r="J15" s="8">
+        <v>9.5999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="B16" s="8">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="C16" s="8">
+        <v>-7.2499999999999995E-2</v>
+      </c>
+      <c r="D16" s="8">
+        <v>-1.0699999999999999E-2</v>
+      </c>
+      <c r="E16" s="8">
+        <v>-0.10630000000000001</v>
+      </c>
+      <c r="F16" s="8">
+        <v>-1.0800000000000001E-2</v>
+      </c>
+      <c r="G16" s="8">
+        <v>-4.1000000000000003E-3</v>
+      </c>
+      <c r="H16" s="8">
+        <v>-0.186</v>
+      </c>
+      <c r="I16" s="8">
+        <v>-8.6499999999999994E-2</v>
+      </c>
+      <c r="J16" s="8">
+        <v>9.7000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="B19" s="8">
+        <v>0.42380000000000001</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0.20660000000000001</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0.44829999999999998</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0.33460000000000001</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.44590000000000002</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.4708</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0.49049999999999999</v>
+      </c>
+      <c r="I19" s="8">
+        <v>1</v>
+      </c>
+      <c r="J19" s="8">
+        <v>0.40339999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="B20" s="8">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0.18429999999999999</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0.44779999999999998</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0.3211</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.46889999999999998</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0.49049999999999999</v>
+      </c>
+      <c r="I20" s="8">
+        <v>1</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0.39250000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="B22" s="8">
+        <v>1.15E-2</v>
+      </c>
+      <c r="C22" s="8">
+        <v>-6.6600000000000006E-2</v>
+      </c>
+      <c r="D22" s="8">
+        <v>-6.8999999999999999E-3</v>
+      </c>
+      <c r="E22" s="8">
+        <v>-0.10630000000000001</v>
+      </c>
+      <c r="F22" s="8">
+        <v>-1.09E-2</v>
+      </c>
+      <c r="G22" s="8">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="H22" s="8">
+        <v>-0.18629999999999999</v>
+      </c>
+      <c r="I22" s="8">
+        <v>-8.2799999999999999E-2</v>
+      </c>
+      <c r="J22" s="8">
+        <v>9.5999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="B23" s="8">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="C23" s="8">
+        <v>-7.2499999999999995E-2</v>
+      </c>
+      <c r="D23" s="8">
+        <v>-1.0699999999999999E-2</v>
+      </c>
+      <c r="E23" s="8">
+        <v>-0.10630000000000001</v>
+      </c>
+      <c r="F23" s="8">
+        <v>-1.0800000000000001E-2</v>
+      </c>
+      <c r="G23" s="8">
+        <v>-4.1000000000000003E-3</v>
+      </c>
+      <c r="H23" s="8">
+        <v>-0.186</v>
+      </c>
+      <c r="I23" s="8">
+        <v>-8.6499999999999994E-2</v>
+      </c>
+      <c r="J23" s="8">
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
   </sheetData>
@@ -11384,7 +12007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update legends in data.
</commit_message>
<xml_diff>
--- a/figs_src/data_all_hpca.xlsx
+++ b/figs_src/data_all_hpca.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7905" yWindow="-15" windowWidth="7980" windowHeight="8970" firstSheet="10" activeTab="12"/>
+    <workbookView xWindow="7905" yWindow="-15" windowWidth="7980" windowHeight="8970" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="full_mon" sheetId="4" r:id="rId1"/>
@@ -262,10 +262,10 @@
     <t>8.0x Overhead Target</t>
   </si>
   <si>
-    <t>4.0x Overhead Target</t>
+    <t>6.0x Overhead Target</t>
   </si>
   <si>
-    <t>6.0x Overhead Target</t>
+    <t>8.0x</t>
   </si>
 </sst>
 </file>
@@ -1402,11 +1402,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153953792"/>
-        <c:axId val="153955328"/>
+        <c:axId val="153958272"/>
+        <c:axId val="153959808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153953792"/>
+        <c:axId val="153958272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1415,7 +1415,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153955328"/>
+        <c:crossAx val="153959808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1423,7 +1423,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153955328"/>
+        <c:axId val="153959808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1454,7 +1454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153953792"/>
+        <c:crossAx val="153958272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1717,11 +1717,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="154034560"/>
-        <c:axId val="154036096"/>
+        <c:axId val="158233344"/>
+        <c:axId val="158234880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154034560"/>
+        <c:axId val="158233344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1730,7 +1730,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="154036096"/>
+        <c:crossAx val="158234880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1738,7 +1738,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154036096"/>
+        <c:axId val="158234880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1761,13 +1761,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154034560"/>
+        <c:crossAx val="158233344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2500,11 +2501,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="154140032"/>
-        <c:axId val="154154112"/>
+        <c:axId val="158334336"/>
+        <c:axId val="153105536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154140032"/>
+        <c:axId val="158334336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2513,7 +2514,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154154112"/>
+        <c:crossAx val="153105536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2521,7 +2522,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154154112"/>
+        <c:axId val="153105536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2551,7 +2552,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154140032"/>
+        <c:crossAx val="158334336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2990,11 +2991,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="154441984"/>
-        <c:axId val="154456064"/>
+        <c:axId val="158640384"/>
+        <c:axId val="158654464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154441984"/>
+        <c:axId val="158640384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3003,7 +3004,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154456064"/>
+        <c:crossAx val="158654464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3011,7 +3012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154456064"/>
+        <c:axId val="158654464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3041,7 +3042,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154441984"/>
+        <c:crossAx val="158640384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3755,11 +3756,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151932288"/>
-        <c:axId val="151946368"/>
+        <c:axId val="152980864"/>
+        <c:axId val="152994944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151932288"/>
+        <c:axId val="152980864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3768,7 +3769,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151946368"/>
+        <c:crossAx val="152994944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3776,7 +3777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151946368"/>
+        <c:axId val="152994944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3814,7 +3815,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151932288"/>
+        <c:crossAx val="152980864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4498,11 +4499,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151897600"/>
-        <c:axId val="151899136"/>
+        <c:axId val="151901696"/>
+        <c:axId val="151903232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151897600"/>
+        <c:axId val="151901696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4522,7 +4523,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="151899136"/>
+        <c:crossAx val="151903232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -4530,7 +4531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151899136"/>
+        <c:axId val="151903232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4568,7 +4569,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151897600"/>
+        <c:crossAx val="151901696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5142,7 +5143,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8.0x Overhead Target</c:v>
+                  <c:v>8.0x</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5243,11 +5244,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="152034688"/>
-        <c:axId val="152040576"/>
+        <c:axId val="153083264"/>
+        <c:axId val="153089152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152034688"/>
+        <c:axId val="153083264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5266,7 +5267,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152040576"/>
+        <c:crossAx val="153089152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5274,7 +5275,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152040576"/>
+        <c:axId val="153089152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5298,14 +5299,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152034688"/>
+        <c:crossAx val="153083264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5979,11 +5979,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153373312"/>
-        <c:axId val="153379200"/>
+        <c:axId val="153312256"/>
+        <c:axId val="153318144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153373312"/>
+        <c:axId val="153312256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6003,7 +6003,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153379200"/>
+        <c:crossAx val="153318144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6011,7 +6011,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153379200"/>
+        <c:axId val="153318144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6035,14 +6035,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153373312"/>
+        <c:crossAx val="153312256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6616,7 +6615,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8.0x Overhead Target</c:v>
+                  <c:v>8.0x</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6717,11 +6716,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="153539712"/>
-        <c:axId val="153541248"/>
+        <c:axId val="153478272"/>
+        <c:axId val="153479808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153539712"/>
+        <c:axId val="153478272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6740,7 +6739,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153541248"/>
+        <c:crossAx val="153479808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6748,7 +6747,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153541248"/>
+        <c:axId val="153479808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6772,14 +6771,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153539712"/>
+        <c:crossAx val="153478272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7153,7 +7151,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.0x Overhead Target</c:v>
+                  <c:v>4.0x</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7253,11 +7251,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153560576"/>
-        <c:axId val="153562112"/>
+        <c:axId val="153496960"/>
+        <c:axId val="153506944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153560576"/>
+        <c:axId val="153496960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7277,7 +7275,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153562112"/>
+        <c:crossAx val="153506944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7285,7 +7283,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153562112"/>
+        <c:axId val="153506944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7313,13 +7311,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153560576"/>
+        <c:crossAx val="153496960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7331,7 +7330,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.32104768611794832"/>
-          <c:y val="0.82574900089572312"/>
+          <c:y val="0.77555293486418164"/>
           <c:w val="0.34929647295702171"/>
           <c:h val="8.6303983982731383E-2"/>
         </c:manualLayout>
@@ -7594,11 +7593,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153788800"/>
-        <c:axId val="153790336"/>
+        <c:axId val="153753856"/>
+        <c:axId val="153796608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153788800"/>
+        <c:axId val="153753856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7607,7 +7606,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153790336"/>
+        <c:crossAx val="153796608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7615,7 +7614,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153790336"/>
+        <c:axId val="153796608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7646,7 +7645,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153788800"/>
+        <c:crossAx val="153753856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7919,11 +7918,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153801856"/>
-        <c:axId val="153803392"/>
+        <c:axId val="153843200"/>
+        <c:axId val="153844736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153801856"/>
+        <c:axId val="153843200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7932,7 +7931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="153803392"/>
+        <c:crossAx val="153844736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7940,7 +7939,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153803392"/>
+        <c:axId val="153844736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.60000000000000009"/>
@@ -7965,13 +7964,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153801856"/>
+        <c:crossAx val="153843200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8032,7 +8032,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="243" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="260" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8044,7 +8044,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="298" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="260" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8104,7 +8104,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="261" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="243" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8128,7 +8128,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="260" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="243" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8140,7 +8140,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="156" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="159" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8164,7 +8164,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="298" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="260" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8459,7 +8459,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="3080926" cy="2179383"/>
+    <xdr:ext cx="2927106" cy="2025894"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -8486,7 +8486,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="2927819" cy="2026460"/>
+    <xdr:ext cx="2927106" cy="2025894"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -8621,7 +8621,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="2926839" cy="2025431"/>
+    <xdr:ext cx="3080926" cy="2179383"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -8675,7 +8675,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="2927106" cy="2025894"/>
+    <xdr:ext cx="3080926" cy="2179383"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -8702,7 +8702,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6276731" cy="2173654"/>
+    <xdr:ext cx="6125766" cy="2024063"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -8756,7 +8756,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="2927819" cy="2026460"/>
+    <xdr:ext cx="2927106" cy="2025894"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -11245,7 +11245,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -11832,7 +11832,7 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B22" s="8">
         <f t="shared" ref="B22:J22" si="11">B7-B6</f>
@@ -11885,7 +11885,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -12426,7 +12426,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B16" s="8">
         <f t="shared" ref="B16:K16" si="6">B7-B6</f>
@@ -12471,7 +12471,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12660,7 +12660,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B5" s="13">
         <v>7.0000000000000001E-3</v>
@@ -13017,7 +13017,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="14">
         <f t="shared" ref="B14:K14" si="7">B6</f>
@@ -13075,7 +13075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:J3"/>
     </sheetView>
   </sheetViews>

</xml_diff>